<commit_message>
new version with new roles
git-svn-id: https://by-stsvn.bayer-ag.com/svn/DOC41WEBUI@955 7fa4df38-a670-11e2-8034-c9adf4be1a24
</commit_message>
<xml_diff>
--- a/trunk/DOC41WEBUI/docs/BDS User Registration.xlsx
+++ b/trunk/DOC41WEBUI/docs/BDS User Registration.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\DOC41WEBUI\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F4FCF1-2452-4BAE-86E8-28EA1B16A13C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="36" windowWidth="24120" windowHeight="12336"/>
+    <workbookView xWindow="20052" yWindow="-108" windowWidth="20376" windowHeight="12816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Automatic User Registration BDS" sheetId="1" r:id="rId1"/>
@@ -15,12 +21,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Frank Wiesen</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -35,7 +41,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -50,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -64,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -79,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -94,7 +100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -109,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -123,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -138,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -153,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -168,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -182,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -197,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -212,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -227,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -241,7 +247,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -256,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -271,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0">
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -286,7 +292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0">
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -300,7 +306,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0">
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -315,7 +321,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -330,7 +336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -345,7 +351,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0">
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
       <text>
         <r>
           <rPr>
@@ -359,7 +365,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0">
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -374,7 +380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
       <text>
         <r>
           <rPr>
@@ -389,7 +395,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -404,7 +410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -418,7 +424,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="0">
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -433,7 +439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0">
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -448,7 +454,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
       <text>
         <r>
           <rPr>
@@ -463,7 +469,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
       <text>
         <r>
           <rPr>
@@ -477,7 +483,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0">
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
       <text>
         <r>
           <rPr>
@@ -492,7 +498,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0">
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
       <text>
         <r>
           <rPr>
@@ -507,7 +513,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0">
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000022000000}">
       <text>
         <r>
           <rPr>
@@ -522,7 +528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000023000000}">
       <text>
         <r>
           <rPr>
@@ -536,7 +542,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0">
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
       <text>
         <r>
           <rPr>
@@ -551,7 +557,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0">
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
       <text>
         <r>
           <rPr>
@@ -566,7 +572,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0">
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
       <text>
         <r>
           <rPr>
@@ -581,7 +587,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0">
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
       <text>
         <r>
           <rPr>
@@ -595,7 +601,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0">
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000028000000}">
       <text>
         <r>
           <rPr>
@@ -610,7 +616,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0">
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000029000000}">
       <text>
         <r>
           <rPr>
@@ -625,7 +631,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0">
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002A000000}">
       <text>
         <r>
           <rPr>
@@ -640,7 +646,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0">
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002B000000}">
       <text>
         <r>
           <rPr>
@@ -654,7 +660,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0">
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002C000000}">
       <text>
         <r>
           <rPr>
@@ -674,7 +680,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>LASTNAME</t>
   </si>
@@ -730,14 +736,20 @@
     <t>For any changes of the users properties, assignment of further vendors or password reset, do not use this sheet. Create and describe the required changes in an extra ticket.</t>
   </si>
   <si>
-    <t>BDS now offers multiple roles for users. So in the future, we need additionally to know, which role to assign: "PM Supplier" or "PP/PI Toller". Please note the required role at the description of your ticket.</t>
+    <t>Please note the required role at the description of your ticket.</t>
+  </si>
+  <si>
+    <t>BDS now offers multiple roles for users. So in the future, we need additionally to know, which role to assign: "PM Supplier", "PP/PI Toller", "PP/PI Toller Time Frame" or "QM CMO inbound documents".</t>
+  </si>
+  <si>
+    <t>version 3.0, 2019-10-16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -776,6 +788,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -860,7 +878,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -907,9 +925,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -918,14 +937,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -963,9 +985,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -998,9 +1020,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1033,9 +1072,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1208,8 +1264,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1259,7 +1315,7 @@
       <c r="F2" s="6"/>
       <c r="H2" s="20"/>
     </row>
-    <row r="3" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1268,7 +1324,7 @@
       <c r="F3" s="10"/>
       <c r="H3" s="20"/>
     </row>
-    <row r="4" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -1295,7 +1351,7 @@
       <c r="F6" s="10"/>
       <c r="H6" s="20"/>
     </row>
-    <row r="7" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1303,7 +1359,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1311,7 +1367,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1319,7 +1375,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1327,7 +1383,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1346,13 +1402,13 @@
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
-      <c r="O13" s="21"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
@@ -1365,17 +1421,17 @@
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -1384,16 +1440,33 @@
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="20"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection password="FB2F" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="tuaaeRzDcfEV3Hz7Hdtl/aaInFf4zACJn902slZQLvW3LB6VnB7yDHUyiCf0eCOSraZYQQjyZcVSiY1/E8Lt2g==" saltValue="9dPcBTFdvtoLpLdNF4puHw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -1401,7 +1474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1552,7 +1625,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1568,35 +1641,135 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<p:Policy xmlns:p="office.server.policy" id="" local="true">
-  <p:Name>Document</p:Name>
-  <p:Description/>
-  <p:Statement/>
-  <p:PolicyItems>
-    <p:PolicyItem featureId="Microsoft.Office.RecordsManagement.PolicyFeatures.Expiration" staticId="0x0101|-2126682137" UniqueId="ab3b55e9-aae5-4563-b264-599d7d4a4f77">
-      <p:Name>Retention</p:Name>
-      <p:Description>Automatic scheduling of content for processing, and performing a retention action on content that has reached its due date.</p:Description>
-      <p:CustomData>
-        <Schedules nextStageId="2">
-          <Schedule type="Default">
-            <stages>
-              <data stageId="1">
-                <formula id="Bayer SharePoint Retention Policy 2.1"/>
-                <action type="action" id="Microsoft.Office.RecordsManagement.PolicyFeatures.Expiration.Action.MoveToRecycleBin"/>
-              </data>
-            </stages>
-          </Schedule>
-        </Schedules>
-      </p:CustomData>
-    </p:PolicyItem>
-  </p:PolicyItems>
-</p:Policy>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e941b624-166c-4987-9ed6-d539972f16a8">
+      <Value>208</Value>
+    </TaxCatchAll>
+    <gbbd9102adcd43839cd73b51972a464c xmlns="e941b624-166c-4987-9ed6-d539972f16a8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Short-Term</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6d967203-8346-4b9c-90f8-b3828a3fa508</TermId>
+        </TermInfo>
+      </Terms>
+    </gbbd9102adcd43839cd73b51972a464c>
+    <_dlc_ExpireDateSaved xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_dlc_ExpireDate xmlns="http://schemas.microsoft.com/sharepoint/v3">2018-02-25T12:33:43+00:00</_dlc_ExpireDate>
+    <Project xmlns="42bfdc29-fc3c-4da9-9efa-76eb8dc34c0c">n/a</Project>
+    <Confidentality xmlns="$ListId:Documents;">Internal</Confidentality>
+    <TaxKeywordTaxHTField xmlns="e9701967-4230-4fdc-8654-e5574ec1fe8e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Processes xmlns="42bfdc29-fc3c-4da9-9efa-76eb8dc34c0c">
+      <Value>PLM&amp;C Project Planning</Value>
+    </Processes>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Tools xmlns="42bfdc29-fc3c-4da9-9efa-76eb8dc34c0c">SharePoint</Tools>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="565cbfc7-ed2b-4c6c-a2cb-cf088e9b9574">SPTASKFORCE-329-241</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="565cbfc7-ed2b-4c6c-a2cb-cf088e9b9574">
+      <Url>http://sp-appl-bhc.bayer-ag.com/sites/230043/006/003/004/_layouts/DocIdRedir.aspx?ID=SPTASKFORCE-329-241</Url>
+      <Description>SPTASKFORCE-329-241</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="7c593367-9bb5-4764-945e-f6a26d2260c4" ContentTypeId="0x0101" PreviousValue="false"/>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Microsoft.Office.RecordsManagement.PolicyFeatures.ExpirationEventReceiver</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>101</SequenceNumber>
+    <Assembly>Microsoft.Office.Policy, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.RecordsManagement.Internal.UpdateExpireDate</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Microsoft.Office.RecordsManagement.PolicyFeatures.ExpirationEventReceiver</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>102</SequenceNumber>
+    <Assembly>Microsoft.Office.Policy, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.RecordsManagement.Internal.UpdateExpireDate</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Microsoft.Office.RecordsManagement.PolicyFeatures.ExpirationEventReceiver</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>103</SequenceNumber>
+    <Assembly>Microsoft.Office.Policy, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.RecordsManagement.Internal.UpdateExpireDate</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Microsoft.Office.RecordsManagement.PolicyFeatures.ExpirationEventReceiver</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>104</SequenceNumber>
+    <Assembly>Microsoft.Office.Policy, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.RecordsManagement.Internal.UpdateExpireDate</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Microsoft.Office.RecordsManagement.PolicyFeatures.ExpirationEventReceiver</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10009</Type>
+    <SequenceNumber>105</SequenceNumber>
+    <Assembly>Microsoft.Office.Policy, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.RecordsManagement.Internal.UpdateExpireDate</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1929,134 +2102,34 @@
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Microsoft.Office.RecordsManagement.PolicyFeatures.ExpirationEventReceiver</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>101</SequenceNumber>
-    <Assembly>Microsoft.Office.Policy, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.RecordsManagement.Internal.UpdateExpireDate</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Microsoft.Office.RecordsManagement.PolicyFeatures.ExpirationEventReceiver</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>102</SequenceNumber>
-    <Assembly>Microsoft.Office.Policy, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.RecordsManagement.Internal.UpdateExpireDate</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Microsoft.Office.RecordsManagement.PolicyFeatures.ExpirationEventReceiver</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>103</SequenceNumber>
-    <Assembly>Microsoft.Office.Policy, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.RecordsManagement.Internal.UpdateExpireDate</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Microsoft.Office.RecordsManagement.PolicyFeatures.ExpirationEventReceiver</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>104</SequenceNumber>
-    <Assembly>Microsoft.Office.Policy, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.RecordsManagement.Internal.UpdateExpireDate</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Microsoft.Office.RecordsManagement.PolicyFeatures.ExpirationEventReceiver</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10009</Type>
-    <SequenceNumber>105</SequenceNumber>
-    <Assembly>Microsoft.Office.Policy, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.RecordsManagement.Internal.UpdateExpireDate</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="7c593367-9bb5-4764-945e-f6a26d2260c4" ContentTypeId="0x0101" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e941b624-166c-4987-9ed6-d539972f16a8">
-      <Value>208</Value>
-    </TaxCatchAll>
-    <gbbd9102adcd43839cd73b51972a464c xmlns="e941b624-166c-4987-9ed6-d539972f16a8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Short-Term</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6d967203-8346-4b9c-90f8-b3828a3fa508</TermId>
-        </TermInfo>
-      </Terms>
-    </gbbd9102adcd43839cd73b51972a464c>
-    <_dlc_ExpireDateSaved xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_dlc_ExpireDate xmlns="http://schemas.microsoft.com/sharepoint/v3">2018-02-25T12:33:43+00:00</_dlc_ExpireDate>
-    <Project xmlns="42bfdc29-fc3c-4da9-9efa-76eb8dc34c0c">n/a</Project>
-    <Confidentality xmlns="$ListId:Documents;">Internal</Confidentality>
-    <TaxKeywordTaxHTField xmlns="e9701967-4230-4fdc-8654-e5574ec1fe8e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <Processes xmlns="42bfdc29-fc3c-4da9-9efa-76eb8dc34c0c">
-      <Value>PLM&amp;C Project Planning</Value>
-    </Processes>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Tools xmlns="42bfdc29-fc3c-4da9-9efa-76eb8dc34c0c">SharePoint</Tools>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="565cbfc7-ed2b-4c6c-a2cb-cf088e9b9574">SPTASKFORCE-329-241</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="565cbfc7-ed2b-4c6c-a2cb-cf088e9b9574">
-      <Url>http://sp-appl-bhc.bayer-ag.com/sites/230043/006/003/004/_layouts/DocIdRedir.aspx?ID=SPTASKFORCE-329-241</Url>
-      <Description>SPTASKFORCE-329-241</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<p:Policy xmlns:p="office.server.policy" id="" local="true">
+  <p:Name>Document</p:Name>
+  <p:Description/>
+  <p:Statement/>
+  <p:PolicyItems>
+    <p:PolicyItem featureId="Microsoft.Office.RecordsManagement.PolicyFeatures.Expiration" staticId="0x0101|-2126682137" UniqueId="ab3b55e9-aae5-4563-b264-599d7d4a4f77">
+      <p:Name>Retention</p:Name>
+      <p:Description>Automatic scheduling of content for processing, and performing a retention action on content that has reached its due date.</p:Description>
+      <p:CustomData>
+        <Schedules nextStageId="2">
+          <Schedule type="Default">
+            <stages>
+              <data stageId="1">
+                <formula id="Bayer SharePoint Retention Policy 2.1"/>
+                <action type="action" id="Microsoft.Office.RecordsManagement.PolicyFeatures.Expiration.Action.MoveToRecycleBin"/>
+              </data>
+            </stages>
+          </Schedule>
+        </Schedules>
+      </p:CustomData>
+    </p:PolicyItem>
+  </p:PolicyItems>
+</p:Policy>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2068,17 +2141,30 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CABB123C-3EC9-4F95-B6F2-7E7865FC9E85}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1FC2CB1-DD11-4E91-B9C5-5A68368010C6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="office.server.policy"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e941b624-166c-4987-9ed6-d539972f16a8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="565cbfc7-ed2b-4c6c-a2cb-cf088e9b9574"/>
+    <ds:schemaRef ds:uri="42bfdc29-fc3c-4da9-9efa-76eb8dc34c0c"/>
+    <ds:schemaRef ds:uri="$ListId:Documents;"/>
+    <ds:schemaRef ds:uri="e9701967-4230-4fdc-8654-e5574ec1fe8e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E19613B-35AE-42E0-A612-32D15F68C1A5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8972976-99A4-481E-8A06-2CE17A474841}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2107,30 +2193,17 @@
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8972976-99A4-481E-8A06-2CE17A474841}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E19613B-35AE-42E0-A612-32D15F68C1A5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1FC2CB1-DD11-4E91-B9C5-5A68368010C6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CABB123C-3EC9-4F95-B6F2-7E7865FC9E85}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="42bfdc29-fc3c-4da9-9efa-76eb8dc34c0c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e9701967-4230-4fdc-8654-e5574ec1fe8e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="565cbfc7-ed2b-4c6c-a2cb-cf088e9b9574"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="$ListId:Documents;"/>
-    <ds:schemaRef ds:uri="e941b624-166c-4987-9ed6-d539972f16a8"/>
+    <ds:schemaRef ds:uri="office.server.policy"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
new version, integrates role selection and additional hint sheet for SNOW ticket creation updated list of supported roles
git-svn-id: https://by-stsvn.bayer-ag.com/svn/DOC41WEBUI@958 7fa4df38-a670-11e2-8034-c9adf4be1a24
</commit_message>
<xml_diff>
--- a/trunk/DOC41WEBUI/docs/BDS User Registration.xlsx
+++ b/trunk/DOC41WEBUI/docs/BDS User Registration.xlsx
@@ -8,15 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\DOC41WEBUI\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F4FCF1-2452-4BAE-86E8-28EA1B16A13C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1B62F7-7246-4A5C-97FD-E32C2DF41798}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20052" yWindow="-108" windowWidth="20376" windowHeight="12816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Automatic User Registration BDS" sheetId="1" r:id="rId1"/>
     <sheet name="EXAMPLE" sheetId="2" r:id="rId2"/>
+    <sheet name="Ticket Hints for Service Now" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <definedNames>
+    <definedName name="Role">'Automatic User Registration BDS'!$E$27:$E$31</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -680,7 +692,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>LASTNAME</t>
   </si>
@@ -736,13 +748,83 @@
     <t>For any changes of the users properties, assignment of further vendors or password reset, do not use this sheet. Create and describe the required changes in an extra ticket.</t>
   </si>
   <si>
-    <t>Please note the required role at the description of your ticket.</t>
-  </si>
-  <si>
-    <t>BDS now offers multiple roles for users. So in the future, we need additionally to know, which role to assign: "PM Supplier", "PP/PI Toller", "PP/PI Toller Time Frame" or "QM CMO inbound documents".</t>
-  </si>
-  <si>
-    <t>version 3.0, 2019-10-16</t>
+    <t>PM Supplier</t>
+  </si>
+  <si>
+    <t>PP/PI Toller (by Version)</t>
+  </si>
+  <si>
+    <t>PP/PI Toller by Time Frame</t>
+  </si>
+  <si>
+    <t>QM CMO inbound</t>
+  </si>
+  <si>
+    <t>(please select)</t>
+  </si>
+  <si>
+    <t>Select Initial Role of the new Users:</t>
+  </si>
+  <si>
+    <t>version 3.1, 2019-11-08</t>
+  </si>
+  <si>
+    <t>BBS_W_B_eB-EM-Solutions</t>
+  </si>
+  <si>
+    <t>Assignment-Group:</t>
+  </si>
+  <si>
+    <t>Service-Area:</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Configuration-Item:</t>
+  </si>
+  <si>
+    <t>DOC41</t>
+  </si>
+  <si>
+    <t>Category:</t>
+  </si>
+  <si>
+    <t>APPLICATIONS</t>
+  </si>
+  <si>
+    <t>Subcategory</t>
+  </si>
+  <si>
+    <t>WEB_APPLICATIONS</t>
+  </si>
+  <si>
+    <t>Short Description:</t>
+  </si>
+  <si>
+    <t>Attachments:</t>
+  </si>
+  <si>
+    <t>(for list of Roles see first sheet)</t>
+  </si>
+  <si>
+    <t>PDF Scan of Training Certificate
+This Excel Sheet (original Sheet, no PDF print)</t>
+  </si>
+  <si>
+    <t>Please create new BDS users with initial Role: …...</t>
+  </si>
+  <si>
+    <t>If you later need more users to be created, use a new sheet containing only the new users to create. Do not just extend the same processed sheet again extended by extra users.</t>
+  </si>
+  <si>
+    <t>Please note the required role at the short description of your ticket. Also select the Role inside this sheet (one of the green selections).</t>
+  </si>
+  <si>
+    <t>See also the "EXAMPLE" sheet as well as the "Ticket Hints for Service Now".</t>
+  </si>
+  <si>
+    <t>BDS now offers multiple roles for users. So in the future, we need additionally to know, which role to assign: "PM Supplier", "PP/PI Toller (by Version)", "PP/PI Toller Time Frame" or "QM CMO inbound".</t>
   </si>
 </sst>
 </file>
@@ -796,7 +878,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -818,6 +900,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -878,7 +966,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -926,6 +1014,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -933,6 +1037,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -942,6 +1051,306 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" checked="Checked" firstButton="1" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Radio" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2385060</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>30480</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2598420</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1085" name="Option Button 61" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1085"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="13"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="8"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2385060</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>22860</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2598420</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1091" name="Option Button 67" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1091"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000043040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="00FF00" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="11"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="8"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2385060</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>15240</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2598420</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1092" name="Option Button 68" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1092"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000044040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="00FF00" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="11"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="8"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2385060</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2598420</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>167640</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1093" name="Option Button 69" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1093"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000045040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="00FF00" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="11"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="8"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2385060</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>2598420</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>160020</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1094" name="Option Button 70" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1094"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000046040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="00FF00" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="11"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="8"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1265,7 +1674,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1285,7 +1694,7 @@
     <col min="10" max="10" width="83.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1306,7 +1715,7 @@
       </c>
       <c r="H1" s="20"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1315,7 +1724,7 @@
       <c r="F2" s="6"/>
       <c r="H2" s="20"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1324,7 +1733,7 @@
       <c r="F3" s="10"/>
       <c r="H3" s="20"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -1333,7 +1742,7 @@
       <c r="F4" s="10"/>
       <c r="H4" s="20"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1342,7 +1751,7 @@
       <c r="F5" s="10"/>
       <c r="H5" s="20"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1351,7 +1760,7 @@
       <c r="F6" s="10"/>
       <c r="H6" s="20"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1359,7 +1768,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1367,7 +1776,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1375,7 +1784,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1383,7 +1792,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1391,85 +1800,274 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>16</v>
-      </c>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
+      <c r="C13" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>22</v>
+      </c>
       <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
-        <v>17</v>
-      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="21"/>
       <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
+      <c r="D14" s="24" t="s">
+        <v>18</v>
+      </c>
       <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>19</v>
-      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
+      <c r="D15" s="24" t="s">
+        <v>19</v>
+      </c>
       <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
-        <v>18</v>
-      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
+      <c r="D16" s="24" t="s">
+        <v>20</v>
+      </c>
       <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>20</v>
-      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="21"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E29" s="23"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E30" s="23"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="tuaaeRzDcfEV3Hz7Hdtl/aaInFf4zACJn902slZQLvW3LB6VnB7yDHUyiCf0eCOSraZYQQjyZcVSiY1/E8Lt2g==" saltValue="9dPcBTFdvtoLpLdNF4puHw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="rkiK0Ti5iUNMg9upMSIpnp21AMg0NbimAqjchxjvBYPJcR4si0ui48sJ0M7KmMEKLLrYL+67EscnOzLrJcCxqQ==" saltValue="tvvbZ3yWf0EGH8kiQeLNQA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1085" r:id="rId4" name="Option Button 61">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2385060</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>30480</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2598420</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1091" r:id="rId5" name="Option Button 67">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2385060</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>22860</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2598420</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>7620</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1092" r:id="rId6" name="Option Button 68">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2385060</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2598420</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1093" r:id="rId7" name="Option Button 69">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2385060</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>7620</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2598420</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>167640</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1094" r:id="rId8" name="Option Button 70">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2385060</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>2598420</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>160020</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 
@@ -1478,7 +2076,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1627,6 +2225,129 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631619EB-7014-43B8-A41F-F510188D12EF}">
+  <dimension ref="B2:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="11.19921875" style="30"/>
+    <col min="3" max="3" width="22.5" style="30" customWidth="1"/>
+    <col min="4" max="4" width="43.8984375" style="30" customWidth="1"/>
+    <col min="5" max="5" width="27.296875" style="30" customWidth="1"/>
+    <col min="6" max="16384" width="11.19921875" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="25"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="25"/>
+      <c r="C4" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="25"/>
+      <c r="C5" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="25"/>
+      <c r="C6" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="25"/>
+      <c r="C7" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="25"/>
+      <c r="C8" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="25"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+    </row>
+    <row r="10" spans="2:6" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B10" s="25"/>
+      <c r="C10" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2143,20 +2864,20 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1FC2CB1-DD11-4E91-B9C5-5A68368010C6}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="e941b624-166c-4987-9ed6-d539972f16a8"/>
+    <ds:schemaRef ds:uri="e9701967-4230-4fdc-8654-e5574ec1fe8e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="565cbfc7-ed2b-4c6c-a2cb-cf088e9b9574"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e941b624-166c-4987-9ed6-d539972f16a8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="565cbfc7-ed2b-4c6c-a2cb-cf088e9b9574"/>
     <ds:schemaRef ds:uri="42bfdc29-fc3c-4da9-9efa-76eb8dc34c0c"/>
     <ds:schemaRef ds:uri="$ListId:Documents;"/>
-    <ds:schemaRef ds:uri="e9701967-4230-4fdc-8654-e5574ec1fe8e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>